<commit_message>
fumbled my way through 7.rs
</commit_message>
<xml_diff>
--- a/daily_coding_problems.xlsx
+++ b/daily_coding_problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/broderickschipp/Documents/Obsidian Vault/Daily Coding Problems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3683800-0E65-2441-84F7-A1B802DEF329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77BF579-6549-8945-B1CD-020F2D2EE895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
@@ -3064,9 +3064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1084"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H105" sqref="H105"/>
+    <sheetView topLeftCell="E1" zoomScale="139" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3990,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
@@ -4007,11 +4007,20 @@
         <v>104</v>
       </c>
       <c r="F37" t="s">
-        <v>19</v>
+        <v>82</v>
+      </c>
+      <c r="G37" s="5">
+        <v>46031</v>
+      </c>
+      <c r="H37" s="5">
+        <v>46031</v>
+      </c>
+      <c r="J37" s="5">
+        <v>46031</v>
       </c>
       <c r="O37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
@@ -27873,7 +27882,7 @@
         <v>19</v>
       </c>
       <c r="O1026">
-        <f t="shared" ref="O1026:O1089" si="16">COUNTA(G1026:N1026)</f>
+        <f t="shared" ref="O1026:O1051" si="16">COUNTA(G1026:N1026)</f>
         <v>0</v>
       </c>
     </row>
@@ -29293,9 +29302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -29336,15 +29343,15 @@
       </c>
       <c r="C3">
         <f>COUNTIFS(Problems!B:B,"Easy",Problems!F:F,"Solved")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <f>COUNTIFS(Problems!B:B,"Easy",Problems!F:F,"Not Started")</f>
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E3" s="4">
         <f>IF(B3&gt;0,C3/B3,0)</f>
-        <v>3.9325842696629212E-2</v>
+        <v>4.2134831460674156E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -29399,15 +29406,15 @@
       </c>
       <c r="C6">
         <f>SUM(C3:C5)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <f>SUM(D3:D5)</f>
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E6" s="4">
         <f>IF(B6&gt;0,C6/B6,0)</f>
-        <v>1.3850415512465374E-2</v>
+        <v>1.4773776546629732E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29428,11 +29435,11 @@
       </c>
       <c r="B10">
         <f>COUNTA(Problems[Python])</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:C18" si="0">B10/$B$18</f>
-        <v>0.25641025641025639</v>
+        <v>0.26190476190476192</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -29445,7 +29452,7 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>0.10256410256410256</v>
+        <v>9.5238095238095233E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -29454,11 +29461,11 @@
       </c>
       <c r="B12">
         <f>COUNTA(Problems[Rust])</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="7">
         <f t="shared" si="0"/>
-        <v>0.38461538461538464</v>
+        <v>0.38095238095238093</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -29471,7 +29478,7 @@
       </c>
       <c r="C13" s="7">
         <f t="shared" si="0"/>
-        <v>5.128205128205128E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -29480,11 +29487,11 @@
       </c>
       <c r="B14">
         <f>COUNTA(Problems[JavaScript])</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="7">
         <f t="shared" si="0"/>
-        <v>0.10256410256410256</v>
+        <v>0.11904761904761904</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -29497,7 +29504,7 @@
       </c>
       <c r="C15" s="7">
         <f t="shared" si="0"/>
-        <v>2.564102564102564E-2</v>
+        <v>2.3809523809523808E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -29510,7 +29517,7 @@
       </c>
       <c r="C16" s="7">
         <f t="shared" si="0"/>
-        <v>2.564102564102564E-2</v>
+        <v>2.3809523809523808E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -29523,7 +29530,7 @@
       </c>
       <c r="C17" s="7">
         <f t="shared" si="0"/>
-        <v>5.128205128205128E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -29532,7 +29539,7 @@
       </c>
       <c r="B18">
         <f>SUM(B10:B17)</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C18" s="7">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
changed project structure a lotta bit; easy_45.rs
</commit_message>
<xml_diff>
--- a/daily_coding_problems.xlsx
+++ b/daily_coding_problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/broderickschipp/Documents/Obsidian Vault/Daily Coding Problems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DE59AF-054A-D644-AE5E-84C5045351AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA53BDB3-EAEA-5942-9B58-4A67F7728364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
@@ -3120,9 +3120,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N385"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3961,7 +3961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
@@ -4287,11 +4287,14 @@
         <v>120</v>
       </c>
       <c r="F45" t="s">
-        <v>18</v>
+        <v>81</v>
+      </c>
+      <c r="J45" s="5">
+        <v>46043</v>
       </c>
       <c r="N45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
@@ -12626,7 +12629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -12669,15 +12672,15 @@
       </c>
       <c r="C3">
         <f>COUNTIFS(Problems!B:B,"Easy",Problems!F:F,"Solved")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <f>COUNTIFS(Problems!B:B,"Easy",Problems!F:F,"Not Started")</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="4">
         <f>IF(B3&gt;0,C3/B3,0)</f>
-        <v>0.184</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -12732,15 +12735,15 @@
       </c>
       <c r="C6">
         <f>SUM(C3:C5)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <f>SUM(D3:D5)</f>
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E6" s="4">
         <f>IF(B6&gt;0,C6/B6,0)</f>
-        <v>7.03125E-2</v>
+        <v>7.2916666666666671E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12765,7 +12768,7 @@
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:C17" si="0">B10/$B$17</f>
-        <v>0.26666666666666666</v>
+        <v>0.26229508196721313</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -12778,7 +12781,7 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+        <v>6.5573770491803282E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -12787,11 +12790,11 @@
       </c>
       <c r="B12">
         <f>COUNTA(Problems[Rust])</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="7">
         <f t="shared" si="0"/>
-        <v>0.41666666666666669</v>
+        <v>0.42622950819672129</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -12804,7 +12807,7 @@
       </c>
       <c r="C13" s="7">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>4.9180327868852458E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -12817,7 +12820,7 @@
       </c>
       <c r="C14" s="7">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>8.1967213114754092E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -12830,7 +12833,7 @@
       </c>
       <c r="C15" s="7">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+        <v>6.5573770491803282E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -12843,7 +12846,7 @@
       </c>
       <c r="C16" s="7">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>4.9180327868852458E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12852,7 +12855,7 @@
       </c>
       <c r="B17">
         <f>SUM(B10:B16)</f>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="7">
         <f t="shared" si="0"/>

</xml_diff>